<commit_message>
first draft of Reno
</commit_message>
<xml_diff>
--- a/network_sim/output.xlsx
+++ b/network_sim/output.xlsx
@@ -444,7 +444,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -455,13 +455,13 @@
         <v>200</v>
       </c>
       <c r="C4">
-        <v>3200</v>
+        <v>4480</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -472,13 +472,13 @@
         <v>300</v>
       </c>
       <c r="C5">
-        <v>3200</v>
+        <v>11520</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -489,13 +489,13 @@
         <v>400</v>
       </c>
       <c r="C6">
-        <v>3200</v>
+        <v>9600</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -506,13 +506,13 @@
         <v>500</v>
       </c>
       <c r="C7">
-        <v>3200</v>
+        <v>19200</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -523,13 +523,13 @@
         <v>600</v>
       </c>
       <c r="C8">
-        <v>3200</v>
+        <v>16000</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -540,13 +540,13 @@
         <v>700</v>
       </c>
       <c r="C9">
-        <v>3200</v>
+        <v>28800</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -557,13 +557,13 @@
         <v>800</v>
       </c>
       <c r="C10">
-        <v>3200</v>
+        <v>22400</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -574,13 +574,13 @@
         <v>900</v>
       </c>
       <c r="C11">
-        <v>3200</v>
+        <v>38400</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -591,13 +591,13 @@
         <v>1000</v>
       </c>
       <c r="C12">
-        <v>3200</v>
+        <v>28160</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -608,13 +608,13 @@
         <v>1100</v>
       </c>
       <c r="C13">
-        <v>3200</v>
+        <v>46080</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -625,13 +625,13 @@
         <v>1200</v>
       </c>
       <c r="C14">
-        <v>3200</v>
+        <v>33920</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -642,13 +642,13 @@
         <v>1300</v>
       </c>
       <c r="C15">
-        <v>3200</v>
+        <v>55680</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -659,13 +659,13 @@
         <v>1400</v>
       </c>
       <c r="C16">
-        <v>3200</v>
+        <v>40320</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -676,13 +676,13 @@
         <v>1500</v>
       </c>
       <c r="C17">
-        <v>3200</v>
+        <v>65280</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -693,13 +693,13 @@
         <v>1600</v>
       </c>
       <c r="C18">
-        <v>3200</v>
+        <v>46720</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -710,13 +710,13 @@
         <v>1700</v>
       </c>
       <c r="C19">
-        <v>3200</v>
+        <v>74880</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -727,13 +727,13 @@
         <v>1800</v>
       </c>
       <c r="C20">
-        <v>3200</v>
+        <v>53120</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -744,13 +744,13 @@
         <v>1900</v>
       </c>
       <c r="C21">
-        <v>3200</v>
+        <v>84480</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -761,13 +761,13 @@
         <v>2000</v>
       </c>
       <c r="C22">
-        <v>2560</v>
+        <v>59520</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -778,13 +778,13 @@
         <v>2100</v>
       </c>
       <c r="C23">
-        <v>3200</v>
+        <v>94080</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -795,13 +795,13 @@
         <v>2200</v>
       </c>
       <c r="C24">
-        <v>3200</v>
+        <v>65920</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -812,13 +812,13 @@
         <v>2300</v>
       </c>
       <c r="C25">
-        <v>3200</v>
+        <v>103680</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -829,13 +829,13 @@
         <v>2400</v>
       </c>
       <c r="C26">
-        <v>3200</v>
+        <v>72320</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -846,13 +846,13 @@
         <v>2500</v>
       </c>
       <c r="C27">
-        <v>3200</v>
+        <v>113280</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -863,13 +863,13 @@
         <v>2600</v>
       </c>
       <c r="C28">
-        <v>3200</v>
+        <v>78720</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -880,13 +880,13 @@
         <v>2700</v>
       </c>
       <c r="C29">
-        <v>3200</v>
+        <v>39680</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -897,13 +897,13 @@
         <v>2800</v>
       </c>
       <c r="C30">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -914,13 +914,13 @@
         <v>2900</v>
       </c>
       <c r="C31">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -931,13 +931,13 @@
         <v>3000</v>
       </c>
       <c r="C32">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -948,13 +948,13 @@
         <v>3100</v>
       </c>
       <c r="C33">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -965,13 +965,13 @@
         <v>3200</v>
       </c>
       <c r="C34">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -982,13 +982,13 @@
         <v>3300</v>
       </c>
       <c r="C35">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -999,13 +999,13 @@
         <v>3400</v>
       </c>
       <c r="C36">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1016,13 +1016,13 @@
         <v>3500</v>
       </c>
       <c r="C37">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1033,13 +1033,13 @@
         <v>3600</v>
       </c>
       <c r="C38">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1050,13 +1050,13 @@
         <v>3700</v>
       </c>
       <c r="C39">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1067,13 +1067,13 @@
         <v>3800</v>
       </c>
       <c r="C40">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1084,13 +1084,13 @@
         <v>3900</v>
       </c>
       <c r="C41">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1101,13 +1101,13 @@
         <v>4000</v>
       </c>
       <c r="C42">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1118,13 +1118,13 @@
         <v>4100</v>
       </c>
       <c r="C43">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1135,13 +1135,13 @@
         <v>4200</v>
       </c>
       <c r="C44">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1152,13 +1152,13 @@
         <v>4300</v>
       </c>
       <c r="C45">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1169,13 +1169,13 @@
         <v>4400</v>
       </c>
       <c r="C46">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1186,13 +1186,13 @@
         <v>4500</v>
       </c>
       <c r="C47">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1203,13 +1203,13 @@
         <v>4600</v>
       </c>
       <c r="C48">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1220,13 +1220,13 @@
         <v>4700</v>
       </c>
       <c r="C49">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1237,13 +1237,13 @@
         <v>4800</v>
       </c>
       <c r="C50">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1254,13 +1254,13 @@
         <v>4900</v>
       </c>
       <c r="C51">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1295,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1309,7 +1309,7 @@
         <v>100</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>2.9</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1323,7 +1323,7 @@
         <v>200</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5.197631445038131</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1337,7 +1337,7 @@
         <v>300</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>7.02286464978477</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -1351,7 +1351,7 @@
         <v>400</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>9.676964161540262</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -1365,7 +1365,7 @@
         <v>500</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>11.48108737366293</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -1379,7 +1379,7 @@
         <v>600</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>14.2840640402846</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -1393,7 +1393,7 @@
         <v>700</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>16.19135853865013</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -1407,7 +1407,7 @@
         <v>800</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>19.08729694930582</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -1421,7 +1421,7 @@
         <v>900</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>21.03383311293605</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -1435,7 +1435,7 @@
         <v>1000</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>23.92804176884484</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -1449,7 +1449,7 @@
         <v>1100</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>25.81912680736002</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -1463,7 +1463,7 @@
         <v>1200</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>28.6833153657839</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -1477,7 +1477,7 @@
         <v>1300</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>30.60714843611165</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
@@ -1491,7 +1491,7 @@
         <v>1400</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>33.50952365744345</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -1505,7 +1505,7 @@
         <v>1500</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>35.4534143544298</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
@@ -1519,7 +1519,7 @@
         <v>1600</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>38.37999394672695</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -1533,7 +1533,7 @@
         <v>1700</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>40.33700142911891</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -1547,7 +1547,7 @@
         <v>1800</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>43.27983505182375</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -1561,7 +1561,7 @@
         <v>1900</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>45.24586785540937</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -1575,7 +1575,7 @@
         <v>2000</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>48.20012264220149</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -1589,7 +1589,7 @@
         <v>2100</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>50.17262140792511</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -1603,7 +1603,7 @@
         <v>2200</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>53.13519850160618</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -1617,7 +1617,7 @@
         <v>2300</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>55.11248372847466</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -1631,7 +1631,7 @@
         <v>2400</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>58.08130799627527</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -1645,7 +1645,7 @@
         <v>2500</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>60.06223339773678</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -1659,7 +1659,7 @@
         <v>2600</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>63.03586447177104</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -1673,7 +1673,7 @@
         <v>2700</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -1687,7 +1687,7 @@
         <v>2800</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
@@ -1701,7 +1701,7 @@
         <v>2900</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
@@ -1715,7 +1715,7 @@
         <v>3000</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
@@ -1729,7 +1729,7 @@
         <v>3100</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
@@ -1743,7 +1743,7 @@
         <v>3200</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
@@ -1757,7 +1757,7 @@
         <v>3300</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -1771,7 +1771,7 @@
         <v>3400</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
@@ -1785,7 +1785,7 @@
         <v>3500</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -1799,7 +1799,7 @@
         <v>3600</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
@@ -1813,7 +1813,7 @@
         <v>3700</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
@@ -1827,7 +1827,7 @@
         <v>3800</v>
       </c>
       <c r="C40">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
@@ -1841,7 +1841,7 @@
         <v>3900</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D41" t="s">
         <v>6</v>
@@ -1855,7 +1855,7 @@
         <v>4000</v>
       </c>
       <c r="C42">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
@@ -1869,7 +1869,7 @@
         <v>4100</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -1883,7 +1883,7 @@
         <v>4200</v>
       </c>
       <c r="C44">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -1897,7 +1897,7 @@
         <v>4300</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -1911,7 +1911,7 @@
         <v>4400</v>
       </c>
       <c r="C46">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
@@ -1925,7 +1925,7 @@
         <v>4500</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D47" t="s">
         <v>6</v>
@@ -1939,7 +1939,7 @@
         <v>4600</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
@@ -1953,7 +1953,7 @@
         <v>4700</v>
       </c>
       <c r="C49">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
@@ -1967,7 +1967,7 @@
         <v>4800</v>
       </c>
       <c r="C50">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
@@ -1981,7 +1981,7 @@
         <v>4900</v>
       </c>
       <c r="C51">
-        <v>4</v>
+        <v>64.0119955810089</v>
       </c>
       <c r="D51" t="s">
         <v>6</v>

</xml_diff>